<commit_message>
EMMM, pin by indicator and dimension in need
</commit_message>
<xml_diff>
--- a/input/OCHA_pop_LMR.xlsx
+++ b/input/OCHA_pop_LMR.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://acted.sharepoint.com/sites/IMPACTHQ-PublicServices-IMPACT-Education/Documents partages/IMPACT - Education/Education - shared folder/PiN/Cluster retreat/PiN session/Data_preparation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://acted-my.sharepoint.com/personal/martina_vit_impact-initiatives_org/Documents/PiN_app_dev/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="290" documentId="8_{D63770E9-8D5C-4F2A-BD7D-98D3C6683B73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A7184F06-A0BA-487C-A2DB-E4185E34999A}"/>
+  <xr:revisionPtr revIDLastSave="291" documentId="8_{D63770E9-8D5C-4F2A-BD7D-98D3C6683B73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0AF251C1-2137-4C78-974F-C86257444908}"/>
   <bookViews>
-    <workbookView xWindow="28635" yWindow="-16320" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{24D09A16-471A-4A7F-BD10-C475AB78837D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{24D09A16-471A-4A7F-BD10-C475AB78837D}"/>
   </bookViews>
   <sheets>
     <sheet name="ocha" sheetId="1" r:id="rId1"/>
@@ -1068,21 +1068,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DA56C02-61B5-41C1-B66B-44B5B6878CC3}">
   <dimension ref="A1:O25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.40625" customWidth="1"/>
-    <col min="2" max="2" width="12.08984375" customWidth="1"/>
-    <col min="3" max="3" width="17.40625" style="10" customWidth="1"/>
-    <col min="4" max="5" width="12.58984375" customWidth="1"/>
-    <col min="6" max="6" width="13.04296875" customWidth="1"/>
-    <col min="9" max="13" width="25.40625" customWidth="1"/>
+    <col min="1" max="1" width="20.42578125" customWidth="1"/>
+    <col min="2" max="2" width="12.140625" customWidth="1"/>
+    <col min="3" max="3" width="17.42578125" style="10" customWidth="1"/>
+    <col min="4" max="5" width="12.5703125" customWidth="1"/>
+    <col min="6" max="6" width="13" customWidth="1"/>
+    <col min="9" max="13" width="25.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="2" customFormat="1" ht="39.4" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:15" s="2" customFormat="1" ht="39.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -1124,7 +1124,7 @@
       </c>
       <c r="N1" s="1"/>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:15" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A2" s="21" t="s">
         <v>19</v>
       </c>
@@ -1164,7 +1164,7 @@
       <c r="M2" s="22"/>
       <c r="O2" s="17"/>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.75">
+    <row r="3" spans="1:15" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A3" s="21" t="s">
         <v>27</v>
       </c>
@@ -1204,7 +1204,7 @@
       <c r="M3" s="22"/>
       <c r="O3" s="18"/>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.75">
+    <row r="4" spans="1:15" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A4" s="21" t="s">
         <v>23</v>
       </c>
@@ -1244,7 +1244,7 @@
       <c r="M4" s="22"/>
       <c r="O4" s="17"/>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.75">
+    <row r="5" spans="1:15" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A5" s="21" t="s">
         <v>21</v>
       </c>
@@ -1284,7 +1284,7 @@
       <c r="M5" s="22"/>
       <c r="O5" s="18"/>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.75">
+    <row r="6" spans="1:15" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A6" s="21" t="s">
         <v>18</v>
       </c>
@@ -1324,7 +1324,7 @@
       <c r="M6" s="22"/>
       <c r="O6" s="17"/>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.75">
+    <row r="7" spans="1:15" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A7" s="21" t="s">
         <v>34</v>
       </c>
@@ -1364,7 +1364,7 @@
       <c r="M7" s="22"/>
       <c r="O7" s="18"/>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.75">
+    <row r="8" spans="1:15" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A8" s="21" t="s">
         <v>29</v>
       </c>
@@ -1404,7 +1404,7 @@
       <c r="M8" s="22"/>
       <c r="O8" s="17"/>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.75">
+    <row r="9" spans="1:15" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A9" s="21" t="s">
         <v>33</v>
       </c>
@@ -1444,7 +1444,7 @@
       <c r="M9" s="22"/>
       <c r="O9" s="18"/>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.75">
+    <row r="10" spans="1:15" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A10" s="21" t="s">
         <v>32</v>
       </c>
@@ -1484,7 +1484,7 @@
       <c r="M10" s="22"/>
       <c r="O10" s="17"/>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.75">
+    <row r="11" spans="1:15" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A11" s="21" t="s">
         <v>28</v>
       </c>
@@ -1524,7 +1524,7 @@
       <c r="M11" s="22"/>
       <c r="O11" s="18"/>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.75">
+    <row r="12" spans="1:15" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A12" s="21" t="s">
         <v>25</v>
       </c>
@@ -1564,7 +1564,7 @@
       <c r="M12" s="22"/>
       <c r="O12" s="17"/>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.75">
+    <row r="13" spans="1:15" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A13" s="21" t="s">
         <v>24</v>
       </c>
@@ -1604,7 +1604,7 @@
       <c r="M13" s="22"/>
       <c r="O13" s="18"/>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.75">
+    <row r="14" spans="1:15" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A14" s="21" t="s">
         <v>30</v>
       </c>
@@ -1644,7 +1644,7 @@
       <c r="M14" s="22"/>
       <c r="O14" s="17"/>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.75">
+    <row r="15" spans="1:15" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A15" s="21" t="s">
         <v>26</v>
       </c>
@@ -1684,7 +1684,7 @@
       <c r="M15" s="22"/>
       <c r="O15" s="18"/>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.75">
+    <row r="16" spans="1:15" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A16" s="21" t="s">
         <v>22</v>
       </c>
@@ -1724,7 +1724,7 @@
       <c r="M16" s="22"/>
       <c r="O16" s="17"/>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.75">
+    <row r="17" spans="1:15" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A17" s="21" t="s">
         <v>35</v>
       </c>
@@ -1764,7 +1764,7 @@
       <c r="M17" s="22"/>
       <c r="O17" s="18"/>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.75">
+    <row r="18" spans="1:15" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A18" s="21" t="s">
         <v>31</v>
       </c>
@@ -1804,7 +1804,7 @@
       <c r="M18" s="22"/>
       <c r="O18" s="17"/>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.75">
+    <row r="19" spans="1:15" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A19" s="21" t="s">
         <v>20</v>
       </c>
@@ -1844,27 +1844,27 @@
       <c r="M19" s="22"/>
       <c r="O19" s="18"/>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.75">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C20" s="17"/>
       <c r="O20" s="17"/>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.75">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C21" s="18"/>
       <c r="O21" s="18"/>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.75">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C22" s="17"/>
       <c r="O22" s="17"/>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.75">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C23" s="18"/>
       <c r="O23" s="18"/>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.75">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C24" s="17"/>
       <c r="O24" s="17"/>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.75">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C25" s="18"/>
       <c r="O25" s="18"/>
     </row>
@@ -1881,18 +1881,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A39D4D79-A7A6-48C8-8509-FD3F2A049ECB}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="57.40625" customWidth="1"/>
-    <col min="2" max="3" width="50.1328125" customWidth="1"/>
-    <col min="4" max="4" width="15.54296875" customWidth="1"/>
+    <col min="1" max="1" width="57.42578125" customWidth="1"/>
+    <col min="2" max="3" width="50.140625" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="106.75" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:4" ht="120" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>15</v>
       </c>
@@ -1903,17 +1903,17 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A2" s="5"/>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="3" spans="1:4" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A3" s="6"/>
       <c r="B3" s="6"/>
       <c r="C3" s="6"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>11</v>
       </c>
@@ -1921,7 +1921,7 @@
       <c r="C5" s="7"/>
       <c r="D5" s="7"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.75">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>12</v>
       </c>
@@ -1935,25 +1935,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b5940141-1bc9-4c17-b1bc-e50f6b2083d6">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C9824523CAB29F4DA646F20BAFE41B4C" ma:contentTypeVersion="12" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="8183b6e3dd2861ff90898c9705e60c3b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b5940141-1bc9-4c17-b1bc-e50f6b2083d6" xmlns:ns3="14cbb838-50ff-4dab-9c3f-cddf75f03c13" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="53c12e9c10231d68d9ff6511fbfe21c6" ns2:_="" ns3:_="">
     <xsd:import namespace="b5940141-1bc9-4c17-b1bc-e50f6b2083d6"/>
@@ -2164,25 +2145,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EF72984C-7CAF-4465-84DC-EB5808DD6359}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="b5940141-1bc9-4c17-b1bc-e50f6b2083d6"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A924EC25-0BE5-46F8-AE2C-6A15A1C7ACC7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b5940141-1bc9-4c17-b1bc-e50f6b2083d6">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C531804F-D035-404F-9763-8F7319A437FC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2199,4 +2181,22 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A924EC25-0BE5-46F8-AE2C-6A15A1C7ACC7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EF72984C-7CAF-4465-84DC-EB5808DD6359}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="b5940141-1bc9-4c17-b1bc-e50f6b2083d6"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>